<commit_message>
update evenementFinSequence et momentDePrise 97e57ef0b17ba9e6fab3a76d566ed344f08572ca
</commit_message>
<xml_diff>
--- a/nr-add-poso-logical-model/ig/StructureDefinition-fr-ligne-prescription.xlsx
+++ b/nr-add-poso-logical-model/ig/StructureDefinition-fr-ligne-prescription.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1406" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1437" uniqueCount="173">
   <si>
     <t>Property</t>
   </si>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-07-15T15:27:28+00:00</t>
+    <t>2025-07-17T07:34:21+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -330,89 +330,95 @@
     <t>Numéro de séquence. La séquence s+1 commence à la fin de la séquence s. En cas de séquences ayant le même numéro, celles-ci se déroulent simultanément.</t>
   </si>
   <si>
-    <t>fr-ligne-prescription.posologie.voieAdministration</t>
-  </si>
-  <si>
-    <t>Voie d'administration du traitement</t>
-  </si>
-  <si>
-    <t>fr-ligne-prescription.posologie.siteAdministration</t>
-  </si>
-  <si>
-    <t>Région anatomique d'administration du traitement</t>
-  </si>
-  <si>
-    <t>fr-ligne-prescription.posologie.quantitePrescrite</t>
-  </si>
-  <si>
-    <t>Quantité de traitement prescrite</t>
-  </si>
-  <si>
-    <t>fr-ligne-prescription.posologie.quantitePrescrite.valeur</t>
-  </si>
-  <si>
-    <t>Quantité à prendre par prise</t>
-  </si>
-  <si>
-    <t>fr-ligne-prescription.posologie.quantitePrescrite.valeurMax</t>
-  </si>
-  <si>
-    <t>Quantité maximale à prendre par prise</t>
-  </si>
-  <si>
-    <t>fr-ligne-prescription.posologie.quantitePrescrite.unite</t>
-  </si>
-  <si>
-    <t>Unité de la quantité prescrite (ex : comprimé, mg, ...)</t>
-  </si>
-  <si>
-    <t>fr-ligne-prescription.posologie.quantiteMaxParPeriode</t>
-  </si>
-  <si>
-    <t>Quantité maximale par unité de temps</t>
-  </si>
-  <si>
-    <t>fr-ligne-prescription.posologie.quantiteMaxParPeriode.valeurQuantite</t>
-  </si>
-  <si>
-    <t>Valeur maximale pour l'unité de temps donnée</t>
-  </si>
-  <si>
-    <t>fr-ligne-prescription.posologie.quantiteMaxParPeriode.uniteQuantite</t>
-  </si>
-  <si>
-    <t>Unité de la quantité</t>
-  </si>
-  <si>
-    <t>fr-ligne-prescription.posologie.quantiteMaxParPeriode.valeurTemps</t>
-  </si>
-  <si>
-    <t>Valeur du temps</t>
-  </si>
-  <si>
-    <t>fr-ligne-prescription.posologie.quantiteMaxParPeriode.uniteTemps</t>
-  </si>
-  <si>
-    <t>Unité de temps</t>
-  </si>
-  <si>
-    <t>fr-ligne-prescription.posologie.evenementDeclenchant</t>
-  </si>
-  <si>
-    <t>Evenement déclenchant de la prise</t>
-  </si>
-  <si>
-    <t>fr-ligne-prescription.posologie.evenementDeclenchant.code</t>
+    <t>fr-ligne-prescription.posologie.evenementFinSequence</t>
   </si>
   <si>
     <t xml:space="preserve">CodeableConcept
 </t>
   </si>
   <si>
-    <t>Code ou texte de l'évènement déclenchant</t>
-  </si>
-  <si>
-    <t>fr-ligne-prescription.posologie.evenementDeclenchant.offset</t>
+    <t>Evenement de fin de la séquence</t>
+  </si>
+  <si>
+    <t>fr-ligne-prescription.posologie.voieAdministration</t>
+  </si>
+  <si>
+    <t>Voie d'administration du traitement</t>
+  </si>
+  <si>
+    <t>fr-ligne-prescription.posologie.siteAdministration</t>
+  </si>
+  <si>
+    <t>Région anatomique d'administration du traitement</t>
+  </si>
+  <si>
+    <t>fr-ligne-prescription.posologie.quantitePrescrite</t>
+  </si>
+  <si>
+    <t>Quantité de traitement prescrite</t>
+  </si>
+  <si>
+    <t>fr-ligne-prescription.posologie.quantitePrescrite.valeur</t>
+  </si>
+  <si>
+    <t>Quantité à prendre par prise</t>
+  </si>
+  <si>
+    <t>fr-ligne-prescription.posologie.quantitePrescrite.valeurMax</t>
+  </si>
+  <si>
+    <t>Quantité maximale à prendre par prise</t>
+  </si>
+  <si>
+    <t>fr-ligne-prescription.posologie.quantitePrescrite.unite</t>
+  </si>
+  <si>
+    <t>Unité de la quantité prescrite (ex : comprimé, mg, ...)</t>
+  </si>
+  <si>
+    <t>fr-ligne-prescription.posologie.quantiteMaxParPeriode</t>
+  </si>
+  <si>
+    <t>Quantité maximale par unité de temps</t>
+  </si>
+  <si>
+    <t>fr-ligne-prescription.posologie.quantiteMaxParPeriode.valeurQuantite</t>
+  </si>
+  <si>
+    <t>Valeur maximale pour l'unité de temps donnée</t>
+  </si>
+  <si>
+    <t>fr-ligne-prescription.posologie.quantiteMaxParPeriode.uniteQuantite</t>
+  </si>
+  <si>
+    <t>Unité de la quantité</t>
+  </si>
+  <si>
+    <t>fr-ligne-prescription.posologie.quantiteMaxParPeriode.valeurTemps</t>
+  </si>
+  <si>
+    <t>Valeur du temps</t>
+  </si>
+  <si>
+    <t>fr-ligne-prescription.posologie.quantiteMaxParPeriode.uniteTemps</t>
+  </si>
+  <si>
+    <t>Unité de temps</t>
+  </si>
+  <si>
+    <t>fr-ligne-prescription.posologie.momentDePrise</t>
+  </si>
+  <si>
+    <t>moment de la prise au cours de la journée (ex : 30 minutes avant le repas)</t>
+  </si>
+  <si>
+    <t>fr-ligne-prescription.posologie.momentDePrise.code</t>
+  </si>
+  <si>
+    <t>Code ou texte du moment de prise</t>
+  </si>
+  <si>
+    <t>fr-ligne-prescription.posologie.momentDePrise.offset</t>
   </si>
   <si>
     <t xml:space="preserve">unsignedInt
@@ -422,7 +428,7 @@
     <t>Temps en minute avant/après l'élément déclenchant</t>
   </si>
   <si>
-    <t>fr-ligne-prescription.posologie.condition</t>
+    <t>fr-ligne-prescription.posologie.conditionDePrise</t>
   </si>
   <si>
     <t>Code ou texte de la condition sous laquelle le traitement doit être pris (ex : en cas de douleurs).</t>
@@ -840,7 +846,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AJ44"/>
+  <dimension ref="A1:AJ45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -2124,13 +2130,13 @@
         <v>20</v>
       </c>
       <c r="K13" t="s" s="2">
-        <v>90</v>
+        <v>104</v>
       </c>
       <c r="L13" t="s" s="2">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="M13" t="s" s="2">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="N13" s="2"/>
       <c r="O13" s="2"/>
@@ -2198,10 +2204,10 @@
     </row>
     <row r="14">
       <c r="A14" t="s" s="2">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B14" t="s" s="2">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" t="s" s="2">
@@ -2227,10 +2233,10 @@
         <v>90</v>
       </c>
       <c r="L14" t="s" s="2">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="M14" t="s" s="2">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="N14" s="2"/>
       <c r="O14" s="2"/>
@@ -2281,7 +2287,7 @@
         <v>20</v>
       </c>
       <c r="AF14" t="s" s="2">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="AG14" t="s" s="2">
         <v>73</v>
@@ -2298,10 +2304,10 @@
     </row>
     <row r="15">
       <c r="A15" t="s" s="2">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B15" t="s" s="2">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" t="s" s="2">
@@ -2312,7 +2318,7 @@
         <v>73</v>
       </c>
       <c r="G15" t="s" s="2">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="H15" t="s" s="2">
         <v>20</v>
@@ -2324,13 +2330,13 @@
         <v>20</v>
       </c>
       <c r="K15" t="s" s="2">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="L15" t="s" s="2">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="M15" t="s" s="2">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="N15" s="2"/>
       <c r="O15" s="2"/>
@@ -2381,13 +2387,13 @@
         <v>20</v>
       </c>
       <c r="AF15" t="s" s="2">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="AG15" t="s" s="2">
         <v>73</v>
       </c>
       <c r="AH15" t="s" s="2">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="AI15" t="s" s="2">
         <v>20</v>
@@ -2398,10 +2404,10 @@
     </row>
     <row r="16">
       <c r="A16" t="s" s="2">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B16" t="s" s="2">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" t="s" s="2">
@@ -2412,7 +2418,7 @@
         <v>73</v>
       </c>
       <c r="G16" t="s" s="2">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="H16" t="s" s="2">
         <v>20</v>
@@ -2424,13 +2430,13 @@
         <v>20</v>
       </c>
       <c r="K16" t="s" s="2">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="L16" t="s" s="2">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="M16" t="s" s="2">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="N16" s="2"/>
       <c r="O16" s="2"/>
@@ -2481,13 +2487,13 @@
         <v>20</v>
       </c>
       <c r="AF16" t="s" s="2">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="AG16" t="s" s="2">
         <v>73</v>
       </c>
       <c r="AH16" t="s" s="2">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="AI16" t="s" s="2">
         <v>20</v>
@@ -2498,10 +2504,10 @@
     </row>
     <row r="17">
       <c r="A17" t="s" s="2">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B17" t="s" s="2">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" t="s" s="2">
@@ -2527,10 +2533,10 @@
         <v>87</v>
       </c>
       <c r="L17" t="s" s="2">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="M17" t="s" s="2">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="N17" s="2"/>
       <c r="O17" s="2"/>
@@ -2581,7 +2587,7 @@
         <v>20</v>
       </c>
       <c r="AF17" t="s" s="2">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="AG17" t="s" s="2">
         <v>73</v>
@@ -2598,10 +2604,10 @@
     </row>
     <row r="18">
       <c r="A18" t="s" s="2">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B18" t="s" s="2">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" t="s" s="2">
@@ -2624,13 +2630,13 @@
         <v>20</v>
       </c>
       <c r="K18" t="s" s="2">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="L18" t="s" s="2">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="M18" t="s" s="2">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="N18" s="2"/>
       <c r="O18" s="2"/>
@@ -2681,7 +2687,7 @@
         <v>20</v>
       </c>
       <c r="AF18" t="s" s="2">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="AG18" t="s" s="2">
         <v>73</v>
@@ -2698,10 +2704,10 @@
     </row>
     <row r="19">
       <c r="A19" t="s" s="2">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B19" t="s" s="2">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" t="s" s="2">
@@ -2712,7 +2718,7 @@
         <v>73</v>
       </c>
       <c r="G19" t="s" s="2">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="H19" t="s" s="2">
         <v>20</v>
@@ -2724,13 +2730,13 @@
         <v>20</v>
       </c>
       <c r="K19" t="s" s="2">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="L19" t="s" s="2">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="M19" t="s" s="2">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="N19" s="2"/>
       <c r="O19" s="2"/>
@@ -2781,13 +2787,13 @@
         <v>20</v>
       </c>
       <c r="AF19" t="s" s="2">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="AG19" t="s" s="2">
         <v>73</v>
       </c>
       <c r="AH19" t="s" s="2">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="AI19" t="s" s="2">
         <v>20</v>
@@ -2798,10 +2804,10 @@
     </row>
     <row r="20">
       <c r="A20" t="s" s="2">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B20" t="s" s="2">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" t="s" s="2">
@@ -2812,7 +2818,7 @@
         <v>73</v>
       </c>
       <c r="G20" t="s" s="2">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="H20" t="s" s="2">
         <v>20</v>
@@ -2824,13 +2830,13 @@
         <v>20</v>
       </c>
       <c r="K20" t="s" s="2">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="L20" t="s" s="2">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="M20" t="s" s="2">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="N20" s="2"/>
       <c r="O20" s="2"/>
@@ -2881,13 +2887,13 @@
         <v>20</v>
       </c>
       <c r="AF20" t="s" s="2">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="AG20" t="s" s="2">
         <v>73</v>
       </c>
       <c r="AH20" t="s" s="2">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="AI20" t="s" s="2">
         <v>20</v>
@@ -2898,10 +2904,10 @@
     </row>
     <row r="21">
       <c r="A21" t="s" s="2">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B21" t="s" s="2">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" t="s" s="2">
@@ -2924,13 +2930,13 @@
         <v>20</v>
       </c>
       <c r="K21" t="s" s="2">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="L21" t="s" s="2">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="M21" t="s" s="2">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="N21" s="2"/>
       <c r="O21" s="2"/>
@@ -2981,7 +2987,7 @@
         <v>20</v>
       </c>
       <c r="AF21" t="s" s="2">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="AG21" t="s" s="2">
         <v>73</v>
@@ -2998,10 +3004,10 @@
     </row>
     <row r="22">
       <c r="A22" t="s" s="2">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B22" t="s" s="2">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" t="s" s="2">
@@ -3024,13 +3030,13 @@
         <v>20</v>
       </c>
       <c r="K22" t="s" s="2">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="L22" t="s" s="2">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="M22" t="s" s="2">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="N22" s="2"/>
       <c r="O22" s="2"/>
@@ -3081,7 +3087,7 @@
         <v>20</v>
       </c>
       <c r="AF22" t="s" s="2">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="AG22" t="s" s="2">
         <v>73</v>
@@ -3098,10 +3104,10 @@
     </row>
     <row r="23">
       <c r="A23" t="s" s="2">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B23" t="s" s="2">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" t="s" s="2">
@@ -3124,13 +3130,13 @@
         <v>20</v>
       </c>
       <c r="K23" t="s" s="2">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="L23" t="s" s="2">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="M23" t="s" s="2">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="N23" s="2"/>
       <c r="O23" s="2"/>
@@ -3181,7 +3187,7 @@
         <v>20</v>
       </c>
       <c r="AF23" t="s" s="2">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="AG23" t="s" s="2">
         <v>73</v>
@@ -3198,10 +3204,10 @@
     </row>
     <row r="24">
       <c r="A24" t="s" s="2">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B24" t="s" s="2">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" t="s" s="2">
@@ -3212,7 +3218,7 @@
         <v>73</v>
       </c>
       <c r="G24" t="s" s="2">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="H24" t="s" s="2">
         <v>20</v>
@@ -3224,13 +3230,13 @@
         <v>20</v>
       </c>
       <c r="K24" t="s" s="2">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="L24" t="s" s="2">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="M24" t="s" s="2">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="N24" s="2"/>
       <c r="O24" s="2"/>
@@ -3281,13 +3287,13 @@
         <v>20</v>
       </c>
       <c r="AF24" t="s" s="2">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="AG24" t="s" s="2">
         <v>73</v>
       </c>
       <c r="AH24" t="s" s="2">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="AI24" t="s" s="2">
         <v>20</v>
@@ -3298,10 +3304,10 @@
     </row>
     <row r="25">
       <c r="A25" t="s" s="2">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B25" t="s" s="2">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" t="s" s="2">
@@ -3312,7 +3318,7 @@
         <v>73</v>
       </c>
       <c r="G25" t="s" s="2">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="H25" t="s" s="2">
         <v>20</v>
@@ -3324,7 +3330,7 @@
         <v>20</v>
       </c>
       <c r="K25" t="s" s="2">
-        <v>128</v>
+        <v>79</v>
       </c>
       <c r="L25" t="s" s="2">
         <v>129</v>
@@ -3381,13 +3387,13 @@
         <v>20</v>
       </c>
       <c r="AF25" t="s" s="2">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="AG25" t="s" s="2">
         <v>73</v>
       </c>
       <c r="AH25" t="s" s="2">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="AI25" t="s" s="2">
         <v>20</v>
@@ -3424,13 +3430,13 @@
         <v>20</v>
       </c>
       <c r="K26" t="s" s="2">
+        <v>104</v>
+      </c>
+      <c r="L26" t="s" s="2">
         <v>131</v>
       </c>
-      <c r="L26" t="s" s="2">
-        <v>132</v>
-      </c>
       <c r="M26" t="s" s="2">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="N26" s="2"/>
       <c r="O26" s="2"/>
@@ -3498,10 +3504,10 @@
     </row>
     <row r="27">
       <c r="A27" t="s" s="2">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B27" t="s" s="2">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" t="s" s="2">
@@ -3512,7 +3518,7 @@
         <v>73</v>
       </c>
       <c r="G27" t="s" s="2">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="H27" t="s" s="2">
         <v>20</v>
@@ -3524,7 +3530,7 @@
         <v>20</v>
       </c>
       <c r="K27" t="s" s="2">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="L27" t="s" s="2">
         <v>134</v>
@@ -3581,13 +3587,13 @@
         <v>20</v>
       </c>
       <c r="AF27" t="s" s="2">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="AG27" t="s" s="2">
         <v>73</v>
       </c>
       <c r="AH27" t="s" s="2">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="AI27" t="s" s="2">
         <v>20</v>
@@ -3612,7 +3618,7 @@
         <v>73</v>
       </c>
       <c r="G28" t="s" s="2">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="H28" t="s" s="2">
         <v>20</v>
@@ -3624,13 +3630,13 @@
         <v>20</v>
       </c>
       <c r="K28" t="s" s="2">
+        <v>104</v>
+      </c>
+      <c r="L28" t="s" s="2">
         <v>136</v>
       </c>
-      <c r="L28" t="s" s="2">
-        <v>137</v>
-      </c>
       <c r="M28" t="s" s="2">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="N28" s="2"/>
       <c r="O28" s="2"/>
@@ -3687,7 +3693,7 @@
         <v>73</v>
       </c>
       <c r="AH28" t="s" s="2">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="AI28" t="s" s="2">
         <v>20</v>
@@ -3698,10 +3704,10 @@
     </row>
     <row r="29">
       <c r="A29" t="s" s="2">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B29" t="s" s="2">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" t="s" s="2">
@@ -3724,7 +3730,7 @@
         <v>20</v>
       </c>
       <c r="K29" t="s" s="2">
-        <v>79</v>
+        <v>138</v>
       </c>
       <c r="L29" t="s" s="2">
         <v>139</v>
@@ -3781,7 +3787,7 @@
         <v>20</v>
       </c>
       <c r="AF29" t="s" s="2">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="AG29" t="s" s="2">
         <v>73</v>
@@ -3824,7 +3830,7 @@
         <v>20</v>
       </c>
       <c r="K30" t="s" s="2">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="L30" t="s" s="2">
         <v>141</v>
@@ -3924,7 +3930,7 @@
         <v>20</v>
       </c>
       <c r="K31" t="s" s="2">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="L31" t="s" s="2">
         <v>143</v>
@@ -4112,7 +4118,7 @@
         <v>73</v>
       </c>
       <c r="G33" t="s" s="2">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="H33" t="s" s="2">
         <v>20</v>
@@ -4187,7 +4193,7 @@
         <v>73</v>
       </c>
       <c r="AH33" t="s" s="2">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="AI33" t="s" s="2">
         <v>20</v>
@@ -4212,7 +4218,7 @@
         <v>73</v>
       </c>
       <c r="G34" t="s" s="2">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="H34" t="s" s="2">
         <v>20</v>
@@ -4224,13 +4230,13 @@
         <v>20</v>
       </c>
       <c r="K34" t="s" s="2">
+        <v>90</v>
+      </c>
+      <c r="L34" t="s" s="2">
         <v>149</v>
       </c>
-      <c r="L34" t="s" s="2">
-        <v>150</v>
-      </c>
       <c r="M34" t="s" s="2">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="N34" s="2"/>
       <c r="O34" s="2"/>
@@ -4287,7 +4293,7 @@
         <v>73</v>
       </c>
       <c r="AH34" t="s" s="2">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="AI34" t="s" s="2">
         <v>20</v>
@@ -4298,10 +4304,10 @@
     </row>
     <row r="35">
       <c r="A35" t="s" s="2">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B35" t="s" s="2">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" t="s" s="2">
@@ -4324,7 +4330,7 @@
         <v>20</v>
       </c>
       <c r="K35" t="s" s="2">
-        <v>136</v>
+        <v>151</v>
       </c>
       <c r="L35" t="s" s="2">
         <v>152</v>
@@ -4381,7 +4387,7 @@
         <v>20</v>
       </c>
       <c r="AF35" t="s" s="2">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="AG35" t="s" s="2">
         <v>73</v>
@@ -4424,7 +4430,7 @@
         <v>20</v>
       </c>
       <c r="K36" t="s" s="2">
-        <v>79</v>
+        <v>138</v>
       </c>
       <c r="L36" t="s" s="2">
         <v>154</v>
@@ -4524,7 +4530,7 @@
         <v>20</v>
       </c>
       <c r="K37" t="s" s="2">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="L37" t="s" s="2">
         <v>156</v>
@@ -4624,7 +4630,7 @@
         <v>20</v>
       </c>
       <c r="K38" t="s" s="2">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="L38" t="s" s="2">
         <v>158</v>
@@ -4724,7 +4730,7 @@
         <v>20</v>
       </c>
       <c r="K39" t="s" s="2">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="L39" t="s" s="2">
         <v>160</v>
@@ -4824,7 +4830,7 @@
         <v>20</v>
       </c>
       <c r="K40" t="s" s="2">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="L40" t="s" s="2">
         <v>162</v>
@@ -5024,7 +5030,7 @@
         <v>20</v>
       </c>
       <c r="K42" t="s" s="2">
-        <v>79</v>
+        <v>95</v>
       </c>
       <c r="L42" t="s" s="2">
         <v>166</v>
@@ -5124,7 +5130,7 @@
         <v>20</v>
       </c>
       <c r="K43" t="s" s="2">
-        <v>136</v>
+        <v>79</v>
       </c>
       <c r="L43" t="s" s="2">
         <v>168</v>
@@ -5224,7 +5230,7 @@
         <v>20</v>
       </c>
       <c r="K44" t="s" s="2">
-        <v>90</v>
+        <v>138</v>
       </c>
       <c r="L44" t="s" s="2">
         <v>170</v>
@@ -5293,6 +5299,106 @@
         <v>20</v>
       </c>
       <c r="AJ44" t="s" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s" s="2">
+        <v>171</v>
+      </c>
+      <c r="B45" t="s" s="2">
+        <v>171</v>
+      </c>
+      <c r="C45" s="2"/>
+      <c r="D45" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="E45" s="2"/>
+      <c r="F45" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="G45" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="H45" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="I45" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="J45" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="K45" t="s" s="2">
+        <v>90</v>
+      </c>
+      <c r="L45" t="s" s="2">
+        <v>172</v>
+      </c>
+      <c r="M45" t="s" s="2">
+        <v>172</v>
+      </c>
+      <c r="N45" s="2"/>
+      <c r="O45" s="2"/>
+      <c r="P45" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="Q45" s="2"/>
+      <c r="R45" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="S45" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="T45" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="U45" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="V45" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="W45" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="X45" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="Y45" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="Z45" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AA45" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AB45" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AC45" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AD45" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AE45" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AF45" t="s" s="2">
+        <v>171</v>
+      </c>
+      <c r="AG45" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="AH45" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AI45" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AJ45" t="s" s="2">
         <v>20</v>
       </c>
     </row>

</xml_diff>